<commit_message>
Completed: Linest and Plots | Awaiting Error Propagation
</commit_message>
<xml_diff>
--- a/Lab_x2/phsx316labx2.xlsx
+++ b/Lab_x2/phsx316labx2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Lab X2</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Volts - Laser</t>
+  </si>
+  <si>
+    <t>Linest:</t>
   </si>
 </sst>
 </file>
@@ -161,6 +164,4422 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mercury -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Blue</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="404157880"/>
+        <c:axId val="404162192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="404157880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current(nA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404162192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="404162192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404157880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mercury -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Green</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.224</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42899999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="404165328"/>
+        <c:axId val="404168856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="404165328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Current(nA)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404168856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="404168856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404165328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Incandescent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Red</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="453230656"/>
+        <c:axId val="453229480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="453230656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Current(nA)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453229480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="453229480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453230656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Laser</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Diffused</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.216</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94899999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="453229872"/>
+        <c:axId val="397930896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="453229872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Current(nA)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397930896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="397930896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Volts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453229872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -450,8 +4869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,13 +5152,23 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5">
+        <f>LINEST(C3:C8,B3:B8,0,TRUE)</f>
+        <v>3.6108597285067871E-2</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="5">
+        <f>LINEST(E3:E8,B3:B8,0,TRUE)</f>
+        <v>3.0542986425339362E-2</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1053,13 +5482,23 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="B26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5">
+        <f>LINEST(D3:D8,B3:B8,0,TRUE)</f>
+        <v>2.0520361990950222E-2</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="5">
+        <f>LINEST(F3:F8,B3:B8,0,TRUE)</f>
+        <v>2.1696832579185515E-2</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1577,5 +6016,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Half Finished: Error Propagation and Finding of Plank's Constants
</commit_message>
<xml_diff>
--- a/Lab_x2/phsx316labx2.xlsx
+++ b/Lab_x2/phsx316labx2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Lab X2</t>
   </si>
@@ -60,6 +60,66 @@
   <si>
     <t>Slope:</t>
   </si>
+  <si>
+    <t>Error Propagation</t>
+  </si>
+  <si>
+    <t>Exp 1</t>
+  </si>
+  <si>
+    <t>Exp 2</t>
+  </si>
+  <si>
+    <t>Exp 3</t>
+  </si>
+  <si>
+    <t>Exp 4</t>
+  </si>
+  <si>
+    <t>Part 5</t>
+  </si>
+  <si>
+    <t>std(volts)</t>
+  </si>
+  <si>
+    <t>std(work)</t>
+  </si>
+  <si>
+    <t>std(wavelength)</t>
+  </si>
+  <si>
+    <t>dh/dv</t>
+  </si>
+  <si>
+    <t>dh/dlambda</t>
+  </si>
+  <si>
+    <t>dh/dphi</t>
+  </si>
+  <si>
+    <t>avg (volts)</t>
+  </si>
+  <si>
+    <t>avg (work)</t>
+  </si>
+  <si>
+    <t>avg (wavelength)</t>
+  </si>
+  <si>
+    <t>Differential</t>
+  </si>
+  <si>
+    <t>Plank's Constant</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>TINV</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +192,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -171,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -196,6 +262,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4304,16 +4374,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.2935779816513763E-3</c:v>
+                  <c:v>2293577.981651376</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8315018315018315E-3</c:v>
+                  <c:v>1831501.8315018313</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4492753623188406E-3</c:v>
+                  <c:v>1449275.3623188403</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5797788309636651E-3</c:v>
+                  <c:v>1579778.8309636652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10189,10 +10259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10210,9 +10280,15 @@
     <col min="14" max="14" width="19.7109375" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" customWidth="1"/>
     <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -10232,7 +10308,7 @@
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -10276,9 +10352,16 @@
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="R2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -10316,20 +10399,52 @@
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="13">
-        <v>436</v>
+        <f>436*10^-9</f>
+        <v>4.3600000000000004E-7</v>
       </c>
       <c r="N3" s="15">
         <v>0.60746332328767116</v>
       </c>
       <c r="O3" s="16">
         <f>1/M3</f>
-        <v>2.2935779816513763E-3</v>
+        <v>2293577.981651376</v>
       </c>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -10367,20 +10482,54 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="14">
-        <v>546</v>
+        <f>546*10^-9</f>
+        <v>5.4600000000000005E-7</v>
       </c>
       <c r="N4" s="15">
         <v>0.16119207397260277</v>
       </c>
       <c r="O4" s="16">
         <f t="shared" ref="O4:O6" si="2">1/M4</f>
-        <v>1.8315018315018315E-3</v>
+        <v>1831501.8315018313</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="Q4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="2">
+        <f>AVERAGE(C3:C8)</f>
+        <v>0.41550000000000004</v>
+      </c>
+      <c r="S4" s="19"/>
+      <c r="T4" s="13">
+        <f>436*10^-9</f>
+        <v>4.3600000000000004E-7</v>
+      </c>
+      <c r="U4">
+        <f>STDEV(H3:H8)</f>
+        <v>0.27596567985802145</v>
+      </c>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4">
+        <f>M3*(1.602*10^-19)/(3*10^8)</f>
+        <v>2.3282400000000003E-34</v>
+      </c>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19">
+        <f>10*10^-9</f>
+        <v>1E-8</v>
+      </c>
+      <c r="AA4">
+        <f>SQRT((X4*R4)^2+(T4*Z4)^2)</f>
+        <v>4.3600000000000006E-15</v>
+      </c>
+      <c r="AB4">
+        <f>R4*M3*(1.602*10^-19)/(3*10^8)</f>
+        <v>9.6738372000000018E-35</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -10418,20 +10567,54 @@
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="14">
-        <v>690</v>
+        <f>690*10^-9</f>
+        <v>6.9000000000000006E-7</v>
       </c>
       <c r="N5" s="15">
         <v>0.68762428493150685</v>
       </c>
       <c r="O5" s="16">
         <f t="shared" si="2"/>
-        <v>1.4492753623188406E-3</v>
+        <v>1449275.3623188403</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="2">
+        <f>AVERAGE(D3:D8)</f>
+        <v>0.223</v>
+      </c>
+      <c r="S5" s="19"/>
+      <c r="T5" s="14">
+        <f>546*10^-9</f>
+        <v>5.4600000000000005E-7</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U7" si="3">STDEV(H4:H9)</f>
+        <v>0.28014322654438739</v>
+      </c>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5">
+        <f t="shared" ref="X5:X7" si="4">M4*(1.602*10^-19)/(3*10^8)</f>
+        <v>2.9156400000000004E-34</v>
+      </c>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19">
+        <f t="shared" ref="Z5:Z8" si="5">10*10^-9</f>
+        <v>1E-8</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" ref="AA5:AA7" si="6">SQRT((X5*R5)^2)</f>
+        <v>6.5018772000000015E-35</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" ref="AB5:AB7" si="7">R5*M4*(1.602*10^-19)/(3*10^8)</f>
+        <v>6.5018772000000015E-35</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -10469,20 +10652,54 @@
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="14">
-        <v>633</v>
+        <f>633*10^-9</f>
+        <v>6.3300000000000002E-7</v>
       </c>
       <c r="N6" s="15">
         <v>0.53206911232876719</v>
       </c>
       <c r="O6" s="16">
         <f t="shared" si="2"/>
-        <v>1.5797788309636651E-3</v>
+        <v>1579778.8309636652</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="2">
+        <f>AVERAGE(E3:E8)</f>
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="S6" s="19"/>
+      <c r="T6" s="14">
+        <f>690*10^-9</f>
+        <v>6.9000000000000006E-7</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="3"/>
+        <v>0.28098457714228708</v>
+      </c>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6">
+        <f t="shared" si="4"/>
+        <v>3.6846000000000001E-34</v>
+      </c>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19">
+        <f t="shared" si="5"/>
+        <v>1E-8</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="6"/>
+        <v>1.4480478E-34</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="7"/>
+        <v>1.4480478E-34</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -10523,10 +10740,43 @@
       <c r="N7" s="2"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="2">
+        <f>AVERAGE(F3:F8)</f>
+        <v>0.30316666666666664</v>
+      </c>
+      <c r="S7" s="19"/>
+      <c r="T7" s="14">
+        <f>633*10^-9</f>
+        <v>6.3300000000000002E-7</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="3"/>
+        <v>0.30074775479583071</v>
+      </c>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7">
+        <f t="shared" si="4"/>
+        <v>3.3802200000000002E-34</v>
+      </c>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19">
+        <f t="shared" si="5"/>
+        <v>1E-8</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="6"/>
+        <v>1.02477003E-34</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="7"/>
+        <v>1.02477003E-34</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -10567,10 +10817,19 @@
       <c r="N8" s="2"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8">
+        <f>P9*(6.02*10^-19)/(3*10^8)</f>
+        <v>-3.7817959880087303E-31</v>
+      </c>
+      <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -10588,19 +10847,25 @@
       </c>
       <c r="N9" s="2">
         <f>LINEST(O3:O6,N3:N6,0,TRUE)</f>
-        <v>3.0632874297093749E-3</v>
+        <v>3063287.4297093749</v>
       </c>
       <c r="O9" s="17" t="s">
         <v>14</v>
       </c>
       <c r="P9" s="3">
-        <f>INDEX(LINEST(O3:O6,N3:N6),1)</f>
-        <v>-1.8846159408681388E-4</v>
+        <f>INDEX(LINEST(O3:O6,N3:N6),1)/(10^9)</f>
+        <v>-1.884615940868138E-4</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
+      <c r="X9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -10628,14 +10893,21 @@
       </c>
       <c r="N10" s="2">
         <f>INDEX(LINEST(O3:O6,N3:N6),2)</f>
-        <v>1.8822153474629128E-3</v>
+        <v>1882215.3474629126</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
+      <c r="X10">
+        <f>TINV(0.05,9)</f>
+        <v>2.2621571627982053</v>
+      </c>
+      <c r="Y10">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -10655,7 +10927,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -10675,7 +10947,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -10695,7 +10967,7 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -10715,7 +10987,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -10735,7 +11007,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -11542,9 +11814,10 @@
       <c r="K75" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B74:K75"/>
+    <mergeCell ref="R2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Small Fix: Propagation Values
</commit_message>
<xml_diff>
--- a/Lab_x2/phsx316labx2.xlsx
+++ b/Lab_x2/phsx316labx2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Lab X2</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>CC</t>
+  </si>
+  <si>
+    <t>ERRORS</t>
   </si>
 </sst>
 </file>
@@ -10261,8 +10264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10521,12 +10524,12 @@
         <v>1E-8</v>
       </c>
       <c r="AA4">
-        <f>SQRT((X4*R4)^2+(T4*Z4)^2)</f>
-        <v>4.3600000000000006E-15</v>
+        <f>SQRT((X4*R4)^2)</f>
+        <v>9.6738372000000018E-35</v>
       </c>
       <c r="AB4">
-        <f>R4*M3*(1.602*10^-19)/(3*10^8)</f>
-        <v>9.6738372000000018E-35</v>
+        <f>(R4 + C3)*M3*(1.602*10^-19)/(3*10^8)</f>
+        <v>1.1466582000000002E-34</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -10610,8 +10613,8 @@
         <v>6.5018772000000015E-35</v>
       </c>
       <c r="AB5">
-        <f t="shared" ref="AB5:AB7" si="7">R5*M4*(1.602*10^-19)/(3*10^8)</f>
-        <v>6.5018772000000015E-35</v>
+        <f>(R5+D3)*M4*(1.602*10^-19)/(3*10^8)</f>
+        <v>8.2804176000000007E-35</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -10695,8 +10698,8 @@
         <v>1.4480478E-34</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="7"/>
-        <v>1.4480478E-34</v>
+        <f>(R6+E3)*M5*(1.602*10^-19)/(3*10^8)</f>
+        <v>1.8091386E-34</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -10772,8 +10775,8 @@
         <v>1.02477003E-34</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="7"/>
-        <v>1.02477003E-34</v>
+        <f>(R7+F3)*M6*(1.602*10^-19)/(3*10^8)</f>
+        <v>1.1971612499999999E-34</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -10864,6 +10867,9 @@
       <c r="Y9" t="s">
         <v>34</v>
       </c>
+      <c r="AA9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -10905,6 +10911,10 @@
       </c>
       <c r="Y10">
         <v>0.75</v>
+      </c>
+      <c r="AA10">
+        <f>AA4*Y10</f>
+        <v>7.2553779000000014E-35</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -10926,6 +10936,10 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
+      <c r="AA11">
+        <f>AA5*Y10</f>
+        <v>4.8764079000000011E-35</v>
+      </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -10946,6 +10960,10 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
+      <c r="AA12">
+        <f>AA6*Y10</f>
+        <v>1.0860358499999999E-34</v>
+      </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -10966,6 +10984,10 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
+      <c r="AA13">
+        <f>AA7*Y10</f>
+        <v>7.6857752249999991E-35</v>
+      </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>

</xml_diff>